<commit_message>
ppt & data changed
</commit_message>
<xml_diff>
--- a/doc/Data.xlsx
+++ b/doc/Data.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="21495" windowHeight="9570" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="20730" windowHeight="9570" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
   <si>
     <t>Iter</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -118,12 +119,55 @@
     <t>Log16_Test_Acc4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>blobs_lr</t>
+  </si>
+  <si>
+    <t>weight_decay_bias</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>weight_decay_q</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lasso_decay_q</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Acc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Loss</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lr1_lasso_10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>o</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4k_Acc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4k_Loss</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,6 +216,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -182,17 +294,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -211,14 +313,11 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -506,7 +605,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -795,7 +893,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1084,7 +1181,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -1373,25 +1469,16 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="121358976"/>
-        <c:axId val="121361536"/>
+        <c:dLbls/>
+        <c:axId val="89748608"/>
+        <c:axId val="89750528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="121358976"/>
+        <c:axId val="89748608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -1410,22 +1497,19 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121361536"/>
+        <c:crossAx val="89750528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="121361536"/>
+        <c:axId val="89750528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -1445,13 +1529,11 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121358976"/>
+        <c:crossAx val="89748608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1459,15 +1541,13 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1475,17 +1555,7 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1504,15 +1574,11 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1800,7 +1866,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2089,25 +2154,16 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="159594752"/>
-        <c:axId val="161781632"/>
+        <c:dLbls/>
+        <c:axId val="86631168"/>
+        <c:axId val="86633088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="159594752"/>
+        <c:axId val="86631168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -2126,23 +2182,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="161781632"/>
+        <c:crossAx val="86633088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="161781632"/>
+        <c:axId val="86633088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -2161,30 +2213,24 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="159594752"/>
+        <c:crossAx val="86631168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2192,17 +2238,7 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2222,14 +2258,11 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2520,7 +2553,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2800,7 +2832,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -3092,7 +3123,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -3372,7 +3402,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -3664,7 +3693,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
@@ -3956,7 +3984,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="6"/>
@@ -4248,7 +4275,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="7"/>
@@ -4540,25 +4566,16 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="250879360"/>
-        <c:axId val="250897536"/>
+        <c:dLbls/>
+        <c:axId val="87017344"/>
+        <c:axId val="87023616"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="250879360"/>
+        <c:axId val="87017344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -4578,22 +4595,19 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="250897536"/>
+        <c:crossAx val="87023616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="250897536"/>
+        <c:axId val="87023616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -4614,13 +4628,11 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="250879360"/>
+        <c:crossAx val="87017344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4628,15 +4640,13 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4644,17 +4654,7 @@
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -4674,14 +4674,11 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -4960,7 +4957,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -5240,7 +5236,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -5532,7 +5527,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -5824,25 +5818,16 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="254370176"/>
-        <c:axId val="254372096"/>
+        <c:dLbls/>
+        <c:axId val="91327488"/>
+        <c:axId val="88409216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="254370176"/>
+        <c:axId val="91327488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -5862,23 +5847,20 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="254372096"/>
+        <c:crossAx val="88409216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="254372096"/>
+        <c:axId val="88409216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="0.30000000000000004"/>
+          <c:min val="0.3000000000000001"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -5898,13 +5880,11 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="254370176"/>
+        <c:crossAx val="91327488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5912,15 +5892,13 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5928,24 +5906,12 @@
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -6233,7 +6199,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -6522,7 +6487,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -6811,7 +6775,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -7100,7 +7063,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -7389,47 +7351,33 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="154233088"/>
-        <c:axId val="154243840"/>
+        <c:dLbls/>
+        <c:axId val="88443520"/>
+        <c:axId val="88461696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="154233088"/>
+        <c:axId val="88443520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154243840"/>
+        <c:crossAx val="88461696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="154243840"/>
+        <c:axId val="88461696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154233088"/>
+        <c:crossAx val="88443520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7437,15 +7385,13 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7453,24 +7399,12 @@
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -7746,7 +7680,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -8035,7 +7968,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -8324,7 +8256,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -8613,7 +8544,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -8902,63 +8832,46 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="338175872"/>
-        <c:axId val="338177408"/>
+        <c:dLbls/>
+        <c:axId val="88511232"/>
+        <c:axId val="88512768"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="338175872"/>
+        <c:axId val="88511232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="338177408"/>
+        <c:crossAx val="88512768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="338177408"/>
+        <c:axId val="88512768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="338175872"/>
+        <c:crossAx val="88511232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8966,24 +8879,12 @@
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -9259,7 +9160,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -9548,7 +9448,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -9837,7 +9736,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -10126,7 +10024,6 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -10415,63 +10312,46 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="261006848"/>
-        <c:axId val="261008384"/>
+        <c:dLbls/>
+        <c:axId val="91405312"/>
+        <c:axId val="91419392"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="261006848"/>
+        <c:axId val="91405312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="261008384"/>
+        <c:crossAx val="91419392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="261008384"/>
+        <c:axId val="91419392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="261006848"/>
+        <c:crossAx val="91405312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -10712,14 +10592,14 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C7EDCC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -10786,7 +10666,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -10821,7 +10700,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -10997,14 +10875,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Y43"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="Y1" activeCellId="5" sqref="A1:A1048576 C1:C1048576 P1:P1048576 S1:S1048576 V1:V1048576 Y1:Y1048576"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="2" max="2" width="23.875" bestFit="1" customWidth="1"/>
     <col min="3" max="7" width="23.875" customWidth="1"/>
@@ -11026,7 +10904,7 @@
     <col min="25" max="25" width="18.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11103,7 +10981,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:25">
       <c r="A2">
         <v>100</v>
       </c>
@@ -11168,7 +11046,7 @@
         <v>1.7115400000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:25">
       <c r="A3">
         <v>200</v>
       </c>
@@ -11233,7 +11111,7 @@
         <v>1.6436299999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:25">
       <c r="A4">
         <v>300</v>
       </c>
@@ -11298,7 +11176,7 @@
         <v>1.5139100000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:25">
       <c r="A5">
         <v>400</v>
       </c>
@@ -11363,7 +11241,7 @@
         <v>1.4438</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:25">
       <c r="A6">
         <v>500</v>
       </c>
@@ -11440,7 +11318,7 @@
         <v>1.3416699999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:25">
       <c r="A7">
         <v>600</v>
       </c>
@@ -11517,7 +11395,7 @@
         <v>1.27888</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:25">
       <c r="A8">
         <v>700</v>
       </c>
@@ -11594,7 +11472,7 @@
         <v>1.29511</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:25">
       <c r="A9">
         <v>800</v>
       </c>
@@ -11671,7 +11549,7 @@
         <v>1.1917599999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:25">
       <c r="A10">
         <v>900</v>
       </c>
@@ -11748,7 +11626,7 @@
         <v>1.17391</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:25">
       <c r="A11">
         <v>1000</v>
       </c>
@@ -11825,7 +11703,7 @@
         <v>1.1868300000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:25">
       <c r="A12">
         <v>1100</v>
       </c>
@@ -11902,7 +11780,7 @@
         <v>1.1696800000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:25">
       <c r="A13">
         <v>1200</v>
       </c>
@@ -11979,7 +11857,7 @@
         <v>1.1598299999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:25">
       <c r="A14">
         <v>1300</v>
       </c>
@@ -12056,7 +11934,7 @@
         <v>1.0983099999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:25">
       <c r="A15">
         <v>1400</v>
       </c>
@@ -12133,7 +12011,7 @@
         <v>1.0749899999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:25">
       <c r="A16">
         <v>1500</v>
       </c>
@@ -12210,7 +12088,7 @@
         <v>1.0800399999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:25">
       <c r="A17">
         <v>1600</v>
       </c>
@@ -12287,7 +12165,7 @@
         <v>1.02627</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:25">
       <c r="A18">
         <v>1700</v>
       </c>
@@ -12364,7 +12242,7 @@
         <v>1.0628599999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:25">
       <c r="A19">
         <v>1800</v>
       </c>
@@ -12441,7 +12319,7 @@
         <v>1.01112</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:25">
       <c r="A20">
         <v>1900</v>
       </c>
@@ -12518,7 +12396,7 @@
         <v>0.99816499999999997</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:25">
       <c r="A21">
         <v>2000</v>
       </c>
@@ -12595,7 +12473,7 @@
         <v>1.0260199999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:25">
       <c r="A22">
         <v>2100</v>
       </c>
@@ -12672,7 +12550,7 @@
         <v>0.97097800000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:25">
       <c r="A23">
         <v>2200</v>
       </c>
@@ -12749,7 +12627,7 @@
         <v>0.96952000000000005</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:25">
       <c r="A24">
         <v>2300</v>
       </c>
@@ -12826,7 +12704,7 @@
         <v>0.985823</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:25">
       <c r="A25">
         <v>2400</v>
       </c>
@@ -12903,7 +12781,7 @@
         <v>0.95281800000000005</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:25">
       <c r="A26">
         <v>2500</v>
       </c>
@@ -12980,7 +12858,7 @@
         <v>0.96326199999999995</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:25">
       <c r="A27">
         <v>2600</v>
       </c>
@@ -13057,7 +12935,7 @@
         <v>0.939079</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:25">
       <c r="A28">
         <v>2700</v>
       </c>
@@ -13134,7 +13012,7 @@
         <v>0.94086199999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:25">
       <c r="A29">
         <v>2800</v>
       </c>
@@ -13211,7 +13089,7 @@
         <v>0.96377599999999997</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:25">
       <c r="A30">
         <v>2900</v>
       </c>
@@ -13288,7 +13166,7 @@
         <v>0.94803700000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:25">
       <c r="A31">
         <v>3000</v>
       </c>
@@ -13365,7 +13243,7 @@
         <v>0.97191799999999995</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:25">
       <c r="A32">
         <v>3100</v>
       </c>
@@ -13442,7 +13320,7 @@
         <v>0.91268899999999997</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:25">
       <c r="A33">
         <v>3200</v>
       </c>
@@ -13519,7 +13397,7 @@
         <v>0.9506</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:25">
       <c r="A34">
         <v>3300</v>
       </c>
@@ -13596,7 +13474,7 @@
         <v>0.93092900000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:25">
       <c r="A35">
         <v>3400</v>
       </c>
@@ -13673,7 +13551,7 @@
         <v>0.91857599999999995</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:25">
       <c r="A36">
         <v>3500</v>
       </c>
@@ -13750,7 +13628,7 @@
         <v>0.92845999999999995</v>
       </c>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:25">
       <c r="A37">
         <v>3600</v>
       </c>
@@ -13827,7 +13705,7 @@
         <v>0.877834</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:25">
       <c r="A38">
         <v>3700</v>
       </c>
@@ -13904,7 +13782,7 @@
         <v>0.96457099999999996</v>
       </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:25">
       <c r="A39">
         <v>3800</v>
       </c>
@@ -13981,7 +13859,7 @@
         <v>0.96956900000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:25">
       <c r="A40">
         <v>3900</v>
       </c>
@@ -14058,7 +13936,7 @@
         <v>0.91084799999999999</v>
       </c>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:25">
       <c r="A41">
         <v>4000</v>
       </c>
@@ -14135,7 +14013,7 @@
         <v>0.91584299999999996</v>
       </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:25">
       <c r="A42">
         <v>4500</v>
       </c>
@@ -14212,7 +14090,7 @@
         <v>0.79361999999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:25">
       <c r="A43">
         <v>5000</v>
       </c>
@@ -14296,16 +14174,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2">
       <c r="A1">
         <v>100</v>
       </c>
@@ -14313,7 +14191,7 @@
         <v>1.8380000000000001</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>200</v>
       </c>
@@ -14321,7 +14199,7 @@
         <v>1.54399</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>300</v>
       </c>
@@ -14329,7 +14207,7 @@
         <v>1.21025</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>400</v>
       </c>
@@ -14337,7 +14215,7 @@
         <v>1.2250399999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>500</v>
       </c>
@@ -14345,7 +14223,7 @@
         <v>1.40486</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>600</v>
       </c>
@@ -14353,7 +14231,7 @@
         <v>1.22722</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2">
       <c r="A7">
         <v>700</v>
       </c>
@@ -14361,7 +14239,7 @@
         <v>1.2252700000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2">
       <c r="A8">
         <v>800</v>
       </c>
@@ -14369,7 +14247,7 @@
         <v>0.86980999999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2">
       <c r="A9">
         <v>900</v>
       </c>
@@ -14377,7 +14255,7 @@
         <v>1.0119</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2">
       <c r="A10">
         <v>1000</v>
       </c>
@@ -14385,7 +14263,7 @@
         <v>1.0942700000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2">
       <c r="A11">
         <v>1100</v>
       </c>
@@ -14393,7 +14271,7 @@
         <v>1.06179</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:2">
       <c r="A12">
         <v>1200</v>
       </c>
@@ -14401,7 +14279,7 @@
         <v>1.0481499999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:2">
       <c r="A13">
         <v>1300</v>
       </c>
@@ -14409,7 +14287,7 @@
         <v>0.71119299999999996</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:2">
       <c r="A14">
         <v>1400</v>
       </c>
@@ -14417,7 +14295,7 @@
         <v>0.90256899999999995</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:2">
       <c r="A15">
         <v>1500</v>
       </c>
@@ -14425,7 +14303,7 @@
         <v>0.91443099999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:2">
       <c r="A16">
         <v>1600</v>
       </c>
@@ -14433,7 +14311,7 @@
         <v>0.84824699999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:2">
       <c r="A17">
         <v>1700</v>
       </c>
@@ -14441,7 +14319,7 @@
         <v>0.91861700000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:2">
       <c r="A18">
         <v>1800</v>
       </c>
@@ -14449,7 +14327,7 @@
         <v>0.637324</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:2">
       <c r="A19">
         <v>1900</v>
       </c>
@@ -14457,7 +14335,7 @@
         <v>0.81530400000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:2">
       <c r="A20">
         <v>2000</v>
       </c>
@@ -14465,7 +14343,7 @@
         <v>0.83082299999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:2">
       <c r="A21">
         <v>2100</v>
       </c>
@@ -14473,7 +14351,7 @@
         <v>0.79962500000000003</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:2">
       <c r="A22">
         <v>2200</v>
       </c>
@@ -14481,7 +14359,7 @@
         <v>0.86688200000000004</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:2">
       <c r="A23">
         <v>2300</v>
       </c>
@@ -14489,7 +14367,7 @@
         <v>0.54902799999999996</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:2">
       <c r="A24">
         <v>2400</v>
       </c>
@@ -14497,7 +14375,7 @@
         <v>0.80520599999999998</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:2">
       <c r="A25">
         <v>2500</v>
       </c>
@@ -14505,7 +14383,7 @@
         <v>0.743668</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:2">
       <c r="A26">
         <v>2600</v>
       </c>
@@ -14513,7 +14391,7 @@
         <v>0.72719199999999995</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:2">
       <c r="A27">
         <v>2700</v>
       </c>
@@ -14521,7 +14399,7 @@
         <v>0.80559800000000004</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:2">
       <c r="A28">
         <v>2800</v>
       </c>
@@ -14529,7 +14407,7 @@
         <v>0.49884800000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:2">
       <c r="A29">
         <v>2900</v>
       </c>
@@ -14537,7 +14415,7 @@
         <v>0.74312900000000004</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:2">
       <c r="A30">
         <v>3000</v>
       </c>
@@ -14545,7 +14423,7 @@
         <v>0.71632200000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:2">
       <c r="A31">
         <v>3100</v>
       </c>
@@ -14553,7 +14431,7 @@
         <v>0.68742000000000003</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:2">
       <c r="A32">
         <v>3200</v>
       </c>
@@ -14561,7 +14439,7 @@
         <v>0.75489499999999998</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:2">
       <c r="A33">
         <v>3300</v>
       </c>
@@ -14569,7 +14447,7 @@
         <v>0.46958299999999997</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:2">
       <c r="A34">
         <v>3400</v>
       </c>
@@ -14577,7 +14455,7 @@
         <v>0.73646199999999995</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:2">
       <c r="A35">
         <v>3500</v>
       </c>
@@ -14585,7 +14463,7 @@
         <v>0.69908800000000004</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:2">
       <c r="A36">
         <v>3600</v>
       </c>
@@ -14593,7 +14471,7 @@
         <v>0.66128200000000004</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:2">
       <c r="A37">
         <v>3700</v>
       </c>
@@ -14601,7 +14479,7 @@
         <v>0.74506600000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:2">
       <c r="A38">
         <v>3800</v>
       </c>
@@ -14609,7 +14487,7 @@
         <v>0.43353700000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:2">
       <c r="A39">
         <v>3900</v>
       </c>
@@ -14617,7 +14495,7 @@
         <v>0.68332199999999998</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:2">
       <c r="A40">
         <v>4000</v>
       </c>
@@ -14625,7 +14503,7 @@
         <v>0.70272699999999999</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:2">
       <c r="A41">
         <v>4100</v>
       </c>
@@ -14633,7 +14511,7 @@
         <v>0.59489099999999995</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:2">
       <c r="A42">
         <v>4200</v>
       </c>
@@ -14641,7 +14519,7 @@
         <v>0.67361099999999996</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:2">
       <c r="A43">
         <v>4300</v>
       </c>
@@ -14649,7 +14527,7 @@
         <v>0.33901999999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:2">
       <c r="A44">
         <v>4400</v>
       </c>
@@ -14657,7 +14535,7 @@
         <v>0.43901600000000002</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:2">
       <c r="A45">
         <v>4500</v>
       </c>
@@ -14665,7 +14543,7 @@
         <v>0.48141600000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:2">
       <c r="A46">
         <v>4600</v>
       </c>
@@ -14673,7 +14551,7 @@
         <v>0.55011500000000002</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:2">
       <c r="A47">
         <v>4700</v>
       </c>
@@ -14681,7 +14559,7 @@
         <v>0.63587499999999997</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:2">
       <c r="A48">
         <v>4800</v>
       </c>
@@ -14689,7 +14567,7 @@
         <v>0.31819700000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:2">
       <c r="A49">
         <v>4900</v>
       </c>
@@ -14697,7 +14575,7 @@
         <v>0.41874400000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:2">
       <c r="A50">
         <v>5000</v>
       </c>
@@ -14712,12 +14590,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14726,17 +14604,408 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="2" max="2" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2">
+        <v>1E-4</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0.1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2">
+        <v>0.69230000000000003</v>
+      </c>
+      <c r="G2">
+        <v>0.91738799999999998</v>
+      </c>
+      <c r="H2">
+        <v>0.72870000000000001</v>
+      </c>
+      <c r="I2">
+        <v>0.80450100000000002</v>
+      </c>
+      <c r="J2">
+        <f>H2-F2</f>
+        <v>3.6399999999999988E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3">
+        <v>1E-4</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0.1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3">
+        <v>0.68700000000000006</v>
+      </c>
+      <c r="G3">
+        <v>0.96030800000000005</v>
+      </c>
+      <c r="H3">
+        <v>0.7228</v>
+      </c>
+      <c r="I3">
+        <v>0.79825299999999999</v>
+      </c>
+      <c r="J3">
+        <f>H3-F3</f>
+        <v>3.5799999999999943E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4">
+        <v>1E-4</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0.01</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4">
+        <v>0.68989999999999996</v>
+      </c>
+      <c r="G4">
+        <v>0.94877699999999998</v>
+      </c>
+      <c r="H4">
+        <v>0.72250000000000003</v>
+      </c>
+      <c r="I4">
+        <v>0.83743500000000004</v>
+      </c>
+      <c r="J4">
+        <f>H4-F4</f>
+        <v>3.2600000000000073E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5">
+        <v>1E-4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0.1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5">
+        <v>0.70230000000000004</v>
+      </c>
+      <c r="G5">
+        <v>0.89487000000000005</v>
+      </c>
+      <c r="H5">
+        <v>0.72889999999999999</v>
+      </c>
+      <c r="I5">
+        <v>0.80138100000000001</v>
+      </c>
+      <c r="J5">
+        <f>H5-F5</f>
+        <v>2.6599999999999957E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6">
+        <v>1E-4</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0.1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6">
+        <v>0.70230000000000004</v>
+      </c>
+      <c r="G6">
+        <v>0.89487000000000005</v>
+      </c>
+      <c r="H6">
+        <v>0.73470000000000002</v>
+      </c>
+      <c r="I6">
+        <v>0.79603599999999997</v>
+      </c>
+      <c r="J6">
+        <f>H6-F6</f>
+        <v>3.2399999999999984E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7">
+        <v>1E-4</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="G7">
+        <v>1.00549</v>
+      </c>
+      <c r="H7">
+        <v>0.71650000000000003</v>
+      </c>
+      <c r="I7">
+        <v>0.84744699999999995</v>
+      </c>
+      <c r="J7">
+        <f>H7-F7</f>
+        <v>5.5499999999999994E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8">
+        <v>1E-4</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>100</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8">
+        <v>0.66649999999999998</v>
+      </c>
+      <c r="G8">
+        <v>0.98563999999999996</v>
+      </c>
+      <c r="H8">
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="I8">
+        <v>0.87454799999999999</v>
+      </c>
+      <c r="J8">
+        <f>H8-F8</f>
+        <v>4.049999999999998E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9">
+        <v>1E-4</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1000</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0.70289999999999997</v>
+      </c>
+      <c r="G9">
+        <v>0.92627099999999996</v>
+      </c>
+      <c r="H9">
+        <v>0.7339</v>
+      </c>
+      <c r="I9">
+        <v>0.82370299999999996</v>
+      </c>
+      <c r="J9">
+        <f>H9-F9</f>
+        <v>3.1000000000000028E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10">
+        <v>1E-4</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1000</v>
+      </c>
+      <c r="D10">
+        <v>0.1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10">
+        <v>0.7046</v>
+      </c>
+      <c r="G10">
+        <v>0.882046</v>
+      </c>
+      <c r="H10">
+        <v>0.73950000000000005</v>
+      </c>
+      <c r="I10">
+        <v>0.76460799999999995</v>
+      </c>
+      <c r="J10">
+        <f>H10-F10</f>
+        <v>3.4900000000000042E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11">
+        <v>1E-4</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1000</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11">
+        <v>0.63219999999999998</v>
+      </c>
+      <c r="G11">
+        <v>1.06718</v>
+      </c>
+      <c r="H11">
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="I11">
+        <v>0.89364100000000002</v>
+      </c>
+      <c r="J11">
+        <f>H11-F11</f>
+        <v>6.579999999999997E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12">
+        <v>1E-4</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:J12">
+    <sortCondition ref="B1"/>
+  </sortState>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update data & ppt
</commit_message>
<xml_diff>
--- a/doc/Data.xlsx
+++ b/doc/Data.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="45">
   <si>
     <t>Iter</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1463,11 +1463,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="318155760"/>
-        <c:axId val="318274136"/>
+        <c:axId val="326941624"/>
+        <c:axId val="328166896"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="318155760"/>
+        <c:axId val="326941624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1495,12 +1495,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="318274136"/>
+        <c:crossAx val="328166896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="318274136"/>
+        <c:axId val="328166896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1529,7 +1529,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="318155760"/>
+        <c:crossAx val="326941624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2175,11 +2175,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="318229480"/>
-        <c:axId val="318229864"/>
+        <c:axId val="328367176"/>
+        <c:axId val="328367560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="318229480"/>
+        <c:axId val="328367176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2208,12 +2208,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="318229864"/>
+        <c:crossAx val="328367560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="318229864"/>
+        <c:axId val="328367560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2242,7 +2242,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="318229480"/>
+        <c:crossAx val="328367176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4622,11 +4622,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="319124392"/>
-        <c:axId val="319124776"/>
+        <c:axId val="328221744"/>
+        <c:axId val="328251024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="319124392"/>
+        <c:axId val="328221744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4655,12 +4655,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="319124776"/>
+        <c:crossAx val="328251024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="319124776"/>
+        <c:axId val="328251024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4690,7 +4690,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="319124392"/>
+        <c:crossAx val="328221744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5902,11 +5902,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="319137880"/>
-        <c:axId val="318870848"/>
+        <c:axId val="325987432"/>
+        <c:axId val="325987824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="319137880"/>
+        <c:axId val="325987432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5935,12 +5935,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="318870848"/>
+        <c:crossAx val="325987824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="318870848"/>
+        <c:axId val="325987824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.3000000000000001"/>
@@ -5970,7 +5970,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="319137880"/>
+        <c:crossAx val="325987432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7464,11 +7464,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="318871632"/>
-        <c:axId val="318872024"/>
+        <c:axId val="326417928"/>
+        <c:axId val="326418320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="318871632"/>
+        <c:axId val="326417928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7478,12 +7478,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="318872024"/>
+        <c:crossAx val="326418320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="318872024"/>
+        <c:axId val="326418320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7494,7 +7494,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="318871632"/>
+        <c:crossAx val="326417928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8976,11 +8976,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="318874768"/>
-        <c:axId val="318875160"/>
+        <c:axId val="326419496"/>
+        <c:axId val="326419888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="318874768"/>
+        <c:axId val="326419496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8990,12 +8990,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="318875160"/>
+        <c:crossAx val="326419888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="318875160"/>
+        <c:axId val="326419888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9006,7 +9006,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="318874768"/>
+        <c:crossAx val="326419496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10488,11 +10488,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="318875944"/>
-        <c:axId val="318876336"/>
+        <c:axId val="326420672"/>
+        <c:axId val="328376160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="318875944"/>
+        <c:axId val="326420672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10502,12 +10502,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="318876336"/>
+        <c:crossAx val="328376160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="318876336"/>
+        <c:axId val="328376160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10518,7 +10518,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="318875944"/>
+        <c:crossAx val="326420672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -14807,8 +14807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H68" sqref="H68"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -16881,7 +16881,7 @@
         <v>42</v>
       </c>
       <c r="C62">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D62" t="s">
         <v>42</v>
@@ -16994,6 +16994,47 @@
       </c>
       <c r="M65">
         <v>0.75528300000000004</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A66">
+        <v>64</v>
+      </c>
+      <c r="B66">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C66">
+        <v>1</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66" t="s">
+        <v>36</v>
+      </c>
+      <c r="G66">
+        <v>1E-4</v>
+      </c>
+      <c r="H66">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="I66" t="s">
+        <v>41</v>
+      </c>
+      <c r="J66">
+        <v>0.72170000000000001</v>
+      </c>
+      <c r="K66">
+        <v>0.83592599999999995</v>
+      </c>
+      <c r="L66">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="M66">
+        <v>0.729487</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.15">

</xml_diff>